<commit_message>
Add function to populate ecl report summarised
</commit_message>
<xml_diff>
--- a/app/templates/reports/ecl_report_summarised.xlsx
+++ b/app/templates/reports/ecl_report_summarised.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">Dalex Finance</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">ECL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XXX</t>
   </si>
   <si>
     <t xml:space="preserve">Recovery rate</t>
@@ -81,11 +78,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -109,18 +107,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -169,31 +155,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,245 +309,229 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="15.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="1" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D18" s="6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E18" s="6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="F18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="6" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D19" s="6" t="n">
-        <v>4000</v>
-      </c>
-      <c r="E19" s="6" t="n">
-        <v>4000</v>
-      </c>
-      <c r="F19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="D21" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="F21" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>